<commit_message>
MasterScript / UnifiedLaw 1 and 2
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim_Draft_1/Code_of_Laws/UnifiedLawIteration.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim_Draft_1/Code_of_Laws/UnifiedLawIteration.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlg\Dropbox (ASU)\PC\Documents\GitHub\REU_MatlabSim\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim_Draft_1\Code_of_Laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA937FCD-44B7-44EE-9587-11BACC5B7F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDB5B20-D469-49A6-8B98-44B4D478687A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="All Iterations" sheetId="2" r:id="rId2"/>
+    <sheet name="thermal Test" sheetId="3" r:id="rId1"/>
+    <sheet name="General Iteration" sheetId="1" r:id="rId2"/>
+    <sheet name="All Iterations" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="134">
   <si>
     <t>dt</t>
   </si>
@@ -434,6 +435,9 @@
   </si>
   <si>
     <t>[-3000,3000]</t>
+  </si>
+  <si>
+    <t>verboseOutput</t>
   </si>
 </sst>
 </file>
@@ -763,11 +767,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K95"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E91F08D-C6B6-4D19-B8C0-C6E2403BA5C0}">
+  <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -833,7 +837,7 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>40</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -849,7 +853,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -857,50 +861,47 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9">
-        <v>10</v>
+        <v>95</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>101</v>
-      </c>
-      <c r="C10" t="b">
-        <v>1</v>
+        <v>96</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15">
-        <v>2600</v>
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -908,356 +909,311 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>26</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>27</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <v>9.81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
         <v>105</v>
       </c>
-      <c r="C27">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>108</v>
-      </c>
-      <c r="B28" t="s">
-        <v>109</v>
-      </c>
       <c r="C28">
-        <v>-3</v>
-      </c>
-      <c r="D28">
-        <v>-2.5</v>
-      </c>
-      <c r="E28">
-        <v>-2</v>
-      </c>
-      <c r="F28">
-        <v>-1.5</v>
-      </c>
-      <c r="G28">
-        <v>-1</v>
-      </c>
-      <c r="H28">
-        <v>-0.5</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
         <v>0.5</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>110</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>111</v>
       </c>
-      <c r="C29">
+      <c r="C30">
         <v>10</v>
-      </c>
-      <c r="D29">
-        <v>9</v>
-      </c>
-      <c r="E29">
-        <v>8</v>
-      </c>
-      <c r="F29">
-        <v>7</v>
-      </c>
-      <c r="G29">
-        <v>6</v>
-      </c>
-      <c r="H29">
-        <v>5</v>
-      </c>
-      <c r="I29">
-        <v>4</v>
-      </c>
-      <c r="J29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>112</v>
-      </c>
-      <c r="C30">
-        <v>0.5</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C31">
         <v>0.5</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+      <c r="B32" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C34" s="2">
         <v>0.01</v>
       </c>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>114</v>
-      </c>
-      <c r="B34" t="s">
-        <v>100</v>
-      </c>
-      <c r="C34">
-        <v>200</v>
-      </c>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
+      <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B35" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="C35">
-        <v>-6</v>
+        <v>200</v>
       </c>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36">
+        <v>-6</v>
+      </c>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
         <v>32</v>
       </c>
-      <c r="C37">
+      <c r="C38">
         <v>1E-4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>117</v>
-      </c>
-      <c r="B38" t="s">
-        <v>118</v>
-      </c>
-      <c r="C38">
-        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>119</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>120</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <v>-2</v>
-      </c>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
-      <c r="K40" s="5"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
-      <c r="B41" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41">
-        <v>9.9999999999999991E-22</v>
-      </c>
+      <c r="A41" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42">
+        <v>9.9999999999999991E-22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" t="s">
         <v>121</v>
       </c>
-      <c r="C42">
+      <c r="C43">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
         <v>38</v>
       </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45" s="3" t="s">
+      <c r="C45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>39</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A46" s="3"/>
-    </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="3"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>98</v>
       </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+      <c r="C49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>14</v>
-      </c>
-      <c r="B51" t="s">
-        <v>43</v>
-      </c>
-      <c r="C51">
-        <v>1000</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="B52" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C52">
-        <v>10</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B53" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C53">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -1265,21 +1221,21 @@
         <v>20</v>
       </c>
       <c r="B54" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C54">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="B55" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C55">
-        <v>-0.26179938779914941</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -1287,120 +1243,123 @@
         <v>49</v>
       </c>
       <c r="B56" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C56">
-        <v>0.26179938779914941</v>
+        <v>-0.26179938779914941</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>49</v>
+      </c>
+      <c r="B57" t="s">
+        <v>50</v>
+      </c>
+      <c r="C57">
+        <v>0.26179938779914941</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>52</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>51</v>
       </c>
-      <c r="C57">
+      <c r="C58">
         <v>5.7595865315812871</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B58" t="s">
-        <v>53</v>
-      </c>
-      <c r="C58">
-        <v>-1.8429999999999998E-2</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C59">
-        <v>0.37819999999999998</v>
+        <v>-1.8429999999999998E-2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
+        <v>54</v>
+      </c>
+      <c r="C60">
+        <v>0.37819999999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
         <v>55</v>
       </c>
-      <c r="C60">
+      <c r="C61">
         <v>-2.3782000000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>14</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>94</v>
       </c>
-      <c r="C61">
+      <c r="C62">
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B64" t="s">
-        <v>57</v>
-      </c>
-      <c r="C64" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C65" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
+        <v>59</v>
+      </c>
+      <c r="C66" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
         <v>61</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C67" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>65</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>63</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B68" t="s">
-        <v>66</v>
-      </c>
-      <c r="C68" t="b">
-        <v>0</v>
-      </c>
-      <c r="I68" s="4"/>
-      <c r="J68" s="4"/>
-      <c r="K68" s="4"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C69" t="b">
         <v>0</v>
       </c>
+      <c r="I69" s="4"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="4"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C70" t="b">
         <v>0</v>
@@ -1408,15 +1367,15 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C71" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C72" t="b">
         <v>0</v>
@@ -1424,75 +1383,72 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
+        <v>70</v>
+      </c>
+      <c r="C73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
         <v>71</v>
       </c>
-      <c r="C73" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
+      <c r="C74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>122</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B75" t="s">
         <v>103</v>
       </c>
-      <c r="C74" t="b">
+      <c r="C75" t="b">
         <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B75" t="s">
-        <v>123</v>
-      </c>
-      <c r="C75">
-        <v>2500</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
+        <v>123</v>
+      </c>
+      <c r="C76">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
         <v>104</v>
       </c>
-      <c r="C76" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+      <c r="C77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A79" s="1"/>
-      <c r="B79" t="s">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A80" s="1"/>
+      <c r="B80" t="s">
         <v>131</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C80" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B80" t="s">
-        <v>73</v>
-      </c>
-      <c r="C80" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
+        <v>73</v>
+      </c>
+      <c r="C81" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
         <v>75</v>
-      </c>
-      <c r="C81">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>86</v>
-      </c>
-      <c r="B82" t="s">
-        <v>76</v>
       </c>
       <c r="C82">
         <v>50</v>
@@ -1500,13 +1456,13 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="B83" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
@@ -1514,7 +1470,7 @@
         <v>20</v>
       </c>
       <c r="B84" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -1522,13 +1478,13 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B85" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C85">
-        <v>300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
@@ -1536,21 +1492,21 @@
         <v>14</v>
       </c>
       <c r="B86" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C86">
-        <v>550</v>
+        <v>300</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="B87" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C87">
-        <v>3</v>
+        <v>550</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
@@ -1558,63 +1514,74 @@
         <v>90</v>
       </c>
       <c r="B88" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C88">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B89" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C89">
-        <v>1E-3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C90">
-        <v>600</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
+        <v>87</v>
+      </c>
+      <c r="B91" t="s">
+        <v>84</v>
+      </c>
+      <c r="C91">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>88</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B92" t="s">
         <v>85</v>
       </c>
-      <c r="C91">
+      <c r="C92">
         <v>1000</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B94" t="s">
-        <v>92</v>
-      </c>
-      <c r="C94" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
+        <v>92</v>
+      </c>
+      <c r="C95" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
         <v>93</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C96" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1625,6 +1592,876 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K96"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="38.21875" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23">
+        <v>9.81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29">
+        <v>-3</v>
+      </c>
+      <c r="D29">
+        <v>-2.5</v>
+      </c>
+      <c r="E29">
+        <v>-2</v>
+      </c>
+      <c r="F29">
+        <v>-1.5</v>
+      </c>
+      <c r="G29">
+        <v>-1</v>
+      </c>
+      <c r="H29">
+        <v>-0.5</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>9</v>
+      </c>
+      <c r="E30">
+        <v>8</v>
+      </c>
+      <c r="F30">
+        <v>7</v>
+      </c>
+      <c r="G30">
+        <v>6</v>
+      </c>
+      <c r="H30">
+        <v>5</v>
+      </c>
+      <c r="I30">
+        <v>4</v>
+      </c>
+      <c r="J30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32">
+        <v>0.5</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35">
+        <v>200</v>
+      </c>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36">
+        <v>-6</v>
+      </c>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>119</v>
+      </c>
+      <c r="B40" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40">
+        <v>-2</v>
+      </c>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42">
+        <v>9.9999999999999991E-22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B46" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" s="3"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" t="s">
+        <v>43</v>
+      </c>
+      <c r="C52">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>45</v>
+      </c>
+      <c r="B53" t="s">
+        <v>44</v>
+      </c>
+      <c r="C53">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>20</v>
+      </c>
+      <c r="B54" t="s">
+        <v>46</v>
+      </c>
+      <c r="C54">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>49</v>
+      </c>
+      <c r="B56" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56">
+        <v>-0.26179938779914941</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>49</v>
+      </c>
+      <c r="B57" t="s">
+        <v>50</v>
+      </c>
+      <c r="C57">
+        <v>0.26179938779914941</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>52</v>
+      </c>
+      <c r="B58" t="s">
+        <v>51</v>
+      </c>
+      <c r="C58">
+        <v>5.7595865315812871</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>53</v>
+      </c>
+      <c r="C59">
+        <v>-1.8429999999999998E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>54</v>
+      </c>
+      <c r="C60">
+        <v>0.37819999999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>55</v>
+      </c>
+      <c r="C61">
+        <v>-2.3782000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>14</v>
+      </c>
+      <c r="B62" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>57</v>
+      </c>
+      <c r="C65" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>59</v>
+      </c>
+      <c r="C66" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>61</v>
+      </c>
+      <c r="C67" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>65</v>
+      </c>
+      <c r="B68" t="s">
+        <v>63</v>
+      </c>
+      <c r="C68" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>66</v>
+      </c>
+      <c r="C69" t="b">
+        <v>0</v>
+      </c>
+      <c r="I69" s="4"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="4"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>67</v>
+      </c>
+      <c r="C70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>68</v>
+      </c>
+      <c r="C71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>69</v>
+      </c>
+      <c r="C72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>70</v>
+      </c>
+      <c r="C73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>71</v>
+      </c>
+      <c r="C74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>122</v>
+      </c>
+      <c r="B75" t="s">
+        <v>103</v>
+      </c>
+      <c r="C75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>123</v>
+      </c>
+      <c r="C76">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>104</v>
+      </c>
+      <c r="C77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A80" s="1"/>
+      <c r="B80" t="s">
+        <v>131</v>
+      </c>
+      <c r="C80" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>73</v>
+      </c>
+      <c r="C81" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>75</v>
+      </c>
+      <c r="C82">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>86</v>
+      </c>
+      <c r="B83" t="s">
+        <v>76</v>
+      </c>
+      <c r="C83">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>20</v>
+      </c>
+      <c r="B84" t="s">
+        <v>77</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>20</v>
+      </c>
+      <c r="B85" t="s">
+        <v>78</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>14</v>
+      </c>
+      <c r="B86" t="s">
+        <v>79</v>
+      </c>
+      <c r="C86">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>14</v>
+      </c>
+      <c r="B87" t="s">
+        <v>80</v>
+      </c>
+      <c r="C87">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>90</v>
+      </c>
+      <c r="B88" t="s">
+        <v>81</v>
+      </c>
+      <c r="C88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>90</v>
+      </c>
+      <c r="B89" t="s">
+        <v>82</v>
+      </c>
+      <c r="C89">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>83</v>
+      </c>
+      <c r="C90">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>87</v>
+      </c>
+      <c r="B91" t="s">
+        <v>84</v>
+      </c>
+      <c r="C91">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>88</v>
+      </c>
+      <c r="B92" t="s">
+        <v>85</v>
+      </c>
+      <c r="C92">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
+        <v>92</v>
+      </c>
+      <c r="C95" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
+        <v>93</v>
+      </c>
+      <c r="C96" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05F4AA9B-FC66-4A95-B187-34F696BBEB40}">
   <dimension ref="A1:K94"/>
   <sheetViews>

</xml_diff>

<commit_message>
UnifiedLaws for Control v Latest Controller
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim_Draft_1/Code_of_Laws/UnifiedLawIteration.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim_Draft_1/Code_of_Laws/UnifiedLawIteration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlg\Dropbox (ASU)\PC\Documents\GitHub\REU_MatlabSim\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim_Draft_1\Code_of_Laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBFD996-84DA-468D-9393-2859745204CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6819D29-4631-4F1A-8984-80B3CCFBDD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="348" yWindow="300" windowWidth="14292" windowHeight="11940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="1020" windowWidth="14292" windowHeight="11940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Iteration" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="139">
   <si>
     <t>dt</t>
   </si>
@@ -437,6 +437,21 @@
   </si>
   <si>
     <t>verboseOutput</t>
+  </si>
+  <si>
+    <t>Scores</t>
+  </si>
+  <si>
+    <t>How many boxes the map should be divided into</t>
+  </si>
+  <si>
+    <t>mapDivResolution</t>
+  </si>
+  <si>
+    <t>How often to check which divisions have been explored</t>
+  </si>
+  <si>
+    <t>mapDivFrameSkip</t>
   </si>
 </sst>
 </file>
@@ -767,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K96"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -855,7 +870,7 @@
         <v>133</v>
       </c>
       <c r="C8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -886,6 +901,9 @@
       <c r="B12" t="s">
         <v>102</v>
       </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -989,7 +1007,7 @@
         <v>34</v>
       </c>
       <c r="C27" s="2">
-        <v>0.1</v>
+        <v>3000</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -1000,7 +1018,7 @@
         <v>105</v>
       </c>
       <c r="C28">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -1011,27 +1029,6 @@
         <v>109</v>
       </c>
       <c r="C29">
-        <v>-3</v>
-      </c>
-      <c r="D29">
-        <v>-2.5</v>
-      </c>
-      <c r="E29">
-        <v>-2</v>
-      </c>
-      <c r="F29">
-        <v>-1.5</v>
-      </c>
-      <c r="G29">
-        <v>-1</v>
-      </c>
-      <c r="H29">
-        <v>-0.5</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
         <v>0.5</v>
       </c>
     </row>
@@ -1045,34 +1042,13 @@
       <c r="C30">
         <v>10</v>
       </c>
-      <c r="D30">
-        <v>9</v>
-      </c>
-      <c r="E30">
-        <v>8</v>
-      </c>
-      <c r="F30">
-        <v>7</v>
-      </c>
-      <c r="G30">
-        <v>6</v>
-      </c>
-      <c r="H30">
-        <v>5</v>
-      </c>
-      <c r="I30">
-        <v>4</v>
-      </c>
-      <c r="J30">
-        <v>3</v>
-      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>112</v>
       </c>
       <c r="C31">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -1080,10 +1056,7 @@
         <v>113</v>
       </c>
       <c r="C32">
-        <v>0.5</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -1096,7 +1069,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="2">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="D34" s="2"/>
     </row>
@@ -1122,7 +1095,7 @@
         <v>116</v>
       </c>
       <c r="C36">
-        <v>-6</v>
+        <v>-2</v>
       </c>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
@@ -1137,7 +1110,7 @@
         <v>32</v>
       </c>
       <c r="C38">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
@@ -1627,6 +1600,33 @@
       </c>
       <c r="C96" t="s">
         <v>125</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>135</v>
+      </c>
+      <c r="B99" t="s">
+        <v>136</v>
+      </c>
+      <c r="C99">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>137</v>
+      </c>
+      <c r="B100" t="s">
+        <v>138</v>
+      </c>
+      <c r="C100">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>